<commit_message>
Offer service test improvements:  - valid action code for savings with loan simulations  - for methods GetBuildingSavingsDepositSchedule, GetBuildingSavingsPaymentSchedule check if balances fits to response of SimulateBuildingSavings
</commit_message>
<xml_diff>
--- a/Tests/backend/postman/NOBY.testdata.xlsx
+++ b/Tests/backend/postman/NOBY.testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\E_JVANA.DS\Desktop\workspace\BE\CIS\0001\OneSolution\Tests\backend\postman\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9B1731A5-7DB7-45D0-BD33-A47115A3E70C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D933BB7C-5438-4BFC-AC44-983590EFE24B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{EF042308-003A-4D5F-9B64-8EBB3EFFFFCE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="45360" windowHeight="23730" xr2:uid="{EF042308-003A-4D5F-9B64-8EBB3EFFFFCE}"/>
   </bookViews>
   <sheets>
     <sheet name="01-OfferService" sheetId="2" r:id="rId1"/>
@@ -411,8 +411,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAC4E102-AADF-4BEB-861E-E665573F06F1}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -476,7 +476,7 @@
         <v>false</v>
       </c>
       <c r="H2">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -506,7 +506,7 @@
         <v>false</v>
       </c>
       <c r="H3">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -536,7 +536,7 @@
         <v>true</v>
       </c>
       <c r="H4">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -566,7 +566,7 @@
         <v>false</v>
       </c>
       <c r="H5">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -596,7 +596,7 @@
         <v>true</v>
       </c>
       <c r="H6">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -626,7 +626,7 @@
         <v>false</v>
       </c>
       <c r="H7">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -656,7 +656,7 @@
         <v>false</v>
       </c>
       <c r="H8">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -686,7 +686,7 @@
         <v>false</v>
       </c>
       <c r="H9">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -716,7 +716,7 @@
         <v>false</v>
       </c>
       <c r="H10">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -729,7 +729,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4632713-2E06-4BB7-8158-C016EA3C4389}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
@@ -786,7 +786,7 @@
         <v>false</v>
       </c>
       <c r="F2" t="str">
-        <f t="shared" ref="F2:G10" si="0">"false"</f>
+        <f t="shared" ref="F2:G2" si="0">"false"</f>
         <v>false</v>
       </c>
       <c r="G2" t="str">

</xml_diff>